<commit_message>
logic improvement for test 3
</commit_message>
<xml_diff>
--- a/tests/data/fail_03_headers_changed/GTN.xlsx
+++ b/tests/data/fail_03_headers_changed/GTN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\Take Home Task - Alexander\tests\data\fail_03_headers_changed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\payroll_data_validator\tests\data\fail_03_headers_changed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23421D2A-230F-477B-A1C3-2654883FF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB9D2C1-9AD0-4832-9CB1-6F3D87A2CF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
   <si>
     <t>employee_id</t>
   </si>
@@ -687,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +709,53 @@
     <col min="12" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>

</xml_diff>